<commit_message>
Played with Some Formulas
</commit_message>
<xml_diff>
--- a/Power-Query/one-skill-you-should-focus-on.xlsx
+++ b/Power-Query/one-skill-you-should-focus-on.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Chandoo.org\power query\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD20B51-41ED-47CB-959A-9B4C1B086E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Ring of Power" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ring of Power'!$C$4:$G$134</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="277">
   <si>
     <t>One Skill to Rule Them All</t>
   </si>
@@ -865,15 +859,18 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>countblank :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="164" formatCode=";;;"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode=";;;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -930,7 +927,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -953,31 +950,285 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1019,7 +1270,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F92F0C86-81F4-8FF2-79D4-1A937B0920E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F92F0C86-81F4-8FF2-79D4-1A937B0920E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1069,7 +1320,7 @@
         <xdr:cNvPr id="6" name="Group 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{309FA60C-7662-B4AF-5ACD-558406884757}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{309FA60C-7662-B4AF-5ACD-558406884757}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1088,7 +1339,7 @@
           <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{510354BA-3BC3-F805-DA62-1DED2DAEC590}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{510354BA-3BC3-F805-DA62-1DED2DAEC590}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1301,7 +1552,7 @@
           <xdr:cNvPr id="5" name="Graphic 4" descr="Mop and bucket with solid fill">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B37E790-1CFB-2F5B-5525-D53020C28C64}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1B37E790-1CFB-2F5B-5525-D53020C28C64}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1310,13 +1561,13 @@
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
             <a:extLst>
               <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
                 <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
               </a:ext>
               <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" xmlns="" r:embed="rId4"/>
               </a:ext>
             </a:extLst>
           </a:blip>
@@ -1338,6 +1589,20 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="C4:G134" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="C4:G134"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" name="Email" dataDxfId="4"/>
+    <tableColumn id="3" name="Course" dataDxfId="3"/>
+    <tableColumn id="4" name="Registration Date" dataDxfId="2"/>
+    <tableColumn id="5" name="Fee Paid" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1383,7 +1648,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1435,7 +1700,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1629,18 +1894,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE182796-6443-4558-9B87-909B73329DFC}">
-  <dimension ref="A1:S134"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S139"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A121" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1921,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
+      <c r="A1" s="4"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1665,29 +1930,29 @@
       <c r="A3" t="s">
         <v>275</v>
       </c>
-      <c r="S3" s="8">
+      <c r="S3" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>147</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1699,12 +1964,12 @@
       <c r="F5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>153</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1716,12 +1981,12 @@
       <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1733,12 +1998,12 @@
       <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>235</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1750,12 +2015,12 @@
       <c r="F8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>209</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1765,12 +2030,12 @@
         <v>263</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="4">
+      <c r="G9" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>201</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1782,12 +2047,12 @@
       <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="6" t="s">
         <v>139</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1799,12 +2064,12 @@
       <c r="F11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>241</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1816,12 +2081,12 @@
       <c r="F12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>167</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1833,12 +2098,12 @@
       <c r="F13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>183</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1850,12 +2115,12 @@
       <c r="F14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="6" t="s">
         <v>117</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1867,12 +2132,12 @@
       <c r="F15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="6" t="s">
         <v>253</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1884,12 +2149,12 @@
       <c r="F16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>159</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1901,12 +2166,12 @@
       <c r="F17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="6" t="s">
         <v>155</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1918,12 +2183,12 @@
       <c r="F18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="6" t="s">
         <v>195</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1933,12 +2198,12 @@
         <v>263</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="4">
+      <c r="G19" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="6" t="s">
         <v>169</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1950,12 +2215,12 @@
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1965,12 +2230,12 @@
         <v>263</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="4">
+      <c r="G21" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="6" t="s">
         <v>145</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1982,12 +2247,12 @@
       <c r="F22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -1997,12 +2262,12 @@
         <v>263</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="4">
+      <c r="G23" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -2014,12 +2279,12 @@
       <c r="F24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="6" t="s">
         <v>151</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -2031,12 +2296,12 @@
       <c r="F25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -2046,12 +2311,12 @@
         <v>263</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -2063,12 +2328,12 @@
       <c r="F27" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="6" t="s">
         <v>245</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -2078,12 +2343,12 @@
         <v>263</v>
       </c>
       <c r="F28" s="3"/>
-      <c r="G28" s="4">
+      <c r="G28" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="6" t="s">
         <v>251</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -2093,12 +2358,12 @@
         <v>263</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="G29" s="4">
+      <c r="G29" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="6" t="s">
         <v>255</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -2110,12 +2375,12 @@
       <c r="F30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2127,12 +2392,12 @@
       <c r="F31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="6" t="s">
         <v>91</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2144,12 +2409,12 @@
       <c r="F32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="6" t="s">
         <v>143</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -2161,12 +2426,12 @@
       <c r="F33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2178,12 +2443,12 @@
       <c r="F34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -2195,12 +2460,12 @@
       <c r="F35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="6" t="s">
         <v>221</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -2212,12 +2477,12 @@
       <c r="F36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="6" t="s">
         <v>60</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -2229,12 +2494,12 @@
       <c r="F37" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -2246,12 +2511,12 @@
       <c r="F38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="6" t="s">
         <v>187</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2263,12 +2528,12 @@
       <c r="F39" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="6" t="s">
         <v>180</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2280,12 +2545,12 @@
       <c r="F40" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="6" t="s">
         <v>199</v>
       </c>
       <c r="D41" s="3" t="s">
@@ -2297,12 +2562,12 @@
       <c r="F41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="3" t="s">
@@ -2312,12 +2577,12 @@
         <v>263</v>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42" s="4">
+      <c r="G42" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="6" t="s">
         <v>79</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -2327,12 +2592,12 @@
         <v>263</v>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43" s="4" t="s">
+      <c r="G43" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="6" t="s">
         <v>231</v>
       </c>
       <c r="D44" s="3" t="s">
@@ -2344,12 +2609,12 @@
       <c r="F44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="6" t="s">
         <v>83</v>
       </c>
       <c r="D45" s="3" t="s">
@@ -2361,12 +2626,12 @@
       <c r="F45" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D46" s="3" t="s">
@@ -2378,12 +2643,12 @@
       <c r="F46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="6" t="s">
         <v>217</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -2395,12 +2660,12 @@
       <c r="F47" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="6" t="s">
         <v>157</v>
       </c>
       <c r="D48" s="3" t="s">
@@ -2412,12 +2677,12 @@
       <c r="F48" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="6" t="s">
         <v>207</v>
       </c>
       <c r="D49" s="3" t="s">
@@ -2429,12 +2694,12 @@
       <c r="F49" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G49" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D50" s="3" t="s">
@@ -2446,12 +2711,12 @@
       <c r="F50" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G50" s="4">
+      <c r="G50" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="6" t="s">
         <v>213</v>
       </c>
       <c r="D51" s="3" t="s">
@@ -2463,12 +2728,12 @@
       <c r="F51" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="6" t="s">
         <v>193</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -2480,12 +2745,12 @@
       <c r="F52" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="6" t="s">
         <v>141</v>
       </c>
       <c r="D53" s="3" t="s">
@@ -2495,12 +2760,12 @@
         <v>263</v>
       </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="4">
+      <c r="G53" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="6" t="s">
         <v>161</v>
       </c>
       <c r="D54" s="3" t="s">
@@ -2512,12 +2777,12 @@
       <c r="F54" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="G54" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="6" t="s">
         <v>249</v>
       </c>
       <c r="D55" s="3" t="s">
@@ -2529,12 +2794,12 @@
       <c r="F55" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D56" s="3" t="s">
@@ -2546,12 +2811,12 @@
       <c r="F56" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="6" t="s">
         <v>103</v>
       </c>
       <c r="D57" s="3" t="s">
@@ -2563,12 +2828,12 @@
       <c r="F57" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="G57" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="6" t="s">
         <v>259</v>
       </c>
       <c r="D58" s="3" t="s">
@@ -2580,12 +2845,12 @@
       <c r="F58" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="G58" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="6" t="s">
         <v>81</v>
       </c>
       <c r="D59" s="3" t="s">
@@ -2595,12 +2860,12 @@
         <v>263</v>
       </c>
       <c r="F59" s="3"/>
-      <c r="G59" s="4">
+      <c r="G59" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="6" t="s">
         <v>205</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -2612,12 +2877,12 @@
       <c r="F60" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G60" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D61" s="3" t="s">
@@ -2629,12 +2894,12 @@
       <c r="F61" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="6" t="s">
         <v>123</v>
       </c>
       <c r="D62" s="3" t="s">
@@ -2646,12 +2911,12 @@
       <c r="F62" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G62" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D63" s="3" t="s">
@@ -2663,12 +2928,12 @@
       <c r="F63" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G63" s="4">
+      <c r="G63" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D64" s="3" t="s">
@@ -2680,12 +2945,12 @@
       <c r="F64" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G64" s="4" t="s">
+      <c r="G64" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="6" t="s">
         <v>203</v>
       </c>
       <c r="D65" s="3" t="s">
@@ -2697,12 +2962,12 @@
       <c r="F65" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G65" s="4">
+      <c r="G65" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="6" t="s">
         <v>189</v>
       </c>
       <c r="D66" s="3" t="s">
@@ -2714,12 +2979,12 @@
       <c r="F66" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G66" s="4">
+      <c r="G66" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="6" t="s">
         <v>247</v>
       </c>
       <c r="D67" s="3" t="s">
@@ -2731,12 +2996,12 @@
       <c r="F67" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="G67" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D68" s="3" t="s">
@@ -2748,12 +3013,12 @@
       <c r="F68" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G68" s="4">
+      <c r="G68" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="6" t="s">
         <v>131</v>
       </c>
       <c r="D69" s="3" t="s">
@@ -2763,12 +3028,12 @@
         <v>263</v>
       </c>
       <c r="F69" s="3"/>
-      <c r="G69" s="4" t="s">
+      <c r="G69" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="3" t="s">
+      <c r="C70" s="6" t="s">
         <v>239</v>
       </c>
       <c r="D70" s="3" t="s">
@@ -2780,12 +3045,12 @@
       <c r="F70" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G70" s="4" t="s">
+      <c r="G70" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="6" t="s">
         <v>177</v>
       </c>
       <c r="D71" s="3" t="s">
@@ -2797,12 +3062,12 @@
       <c r="F71" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G71" s="4" t="s">
+      <c r="G71" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="3" t="s">
+      <c r="C72" s="6" t="s">
         <v>87</v>
       </c>
       <c r="D72" s="3" t="s">
@@ -2814,12 +3079,12 @@
       <c r="F72" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G72" s="4">
+      <c r="G72" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="6" t="s">
         <v>97</v>
       </c>
       <c r="D73" s="3" t="s">
@@ -2831,12 +3096,12 @@
       <c r="F73" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G73" s="4">
+      <c r="G73" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="6" t="s">
         <v>173</v>
       </c>
       <c r="D74" s="3" t="s">
@@ -2846,12 +3111,12 @@
         <v>263</v>
       </c>
       <c r="F74" s="3"/>
-      <c r="G74" s="4" t="s">
+      <c r="G74" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="6" t="s">
         <v>165</v>
       </c>
       <c r="D75" s="3" t="s">
@@ -2863,12 +3128,12 @@
       <c r="F75" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G75" s="4">
+      <c r="G75" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="6" t="s">
         <v>149</v>
       </c>
       <c r="D76" s="3" t="s">
@@ -2880,12 +3145,12 @@
       <c r="F76" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G76" s="4">
+      <c r="G76" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="6" t="s">
         <v>179</v>
       </c>
       <c r="D77" s="3" t="s">
@@ -2897,12 +3162,12 @@
       <c r="F77" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G77" s="4">
+      <c r="G77" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="6" t="s">
         <v>77</v>
       </c>
       <c r="D78" s="3" t="s">
@@ -2914,12 +3179,12 @@
       <c r="F78" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G78" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D79" s="3" t="s">
@@ -2931,12 +3196,12 @@
       <c r="F79" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G79" s="4">
+      <c r="G79" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="6" t="s">
         <v>137</v>
       </c>
       <c r="D80" s="3" t="s">
@@ -2948,12 +3213,12 @@
       <c r="F80" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G80" s="4" t="s">
+      <c r="G80" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="6" t="s">
         <v>215</v>
       </c>
       <c r="D81" s="3" t="s">
@@ -2965,12 +3230,12 @@
       <c r="F81" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G81" s="4" t="s">
+      <c r="G81" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="6" t="s">
         <v>163</v>
       </c>
       <c r="D82" s="3" t="s">
@@ -2982,12 +3247,12 @@
       <c r="F82" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G82" s="4" t="s">
+      <c r="G82" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="6" t="s">
         <v>185</v>
       </c>
       <c r="D83" s="3" t="s">
@@ -2997,12 +3262,12 @@
         <v>263</v>
       </c>
       <c r="F83" s="3"/>
-      <c r="G83" s="4">
+      <c r="G83" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="6" t="s">
         <v>175</v>
       </c>
       <c r="D84" s="3" t="s">
@@ -3014,12 +3279,12 @@
       <c r="F84" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G84" s="4">
+      <c r="G84" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="6" t="s">
         <v>109</v>
       </c>
       <c r="D85" s="3" t="s">
@@ -3031,12 +3296,12 @@
       <c r="F85" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G85" s="4">
+      <c r="G85" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="3" t="s">
+      <c r="C86" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D86" s="3" t="s">
@@ -3048,12 +3313,12 @@
       <c r="F86" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G86" s="4">
+      <c r="G86" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="6" t="s">
         <v>257</v>
       </c>
       <c r="D87" s="3" t="s">
@@ -3063,12 +3328,12 @@
         <v>263</v>
       </c>
       <c r="F87" s="3"/>
-      <c r="G87" s="4">
+      <c r="G87" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="6" t="s">
         <v>171</v>
       </c>
       <c r="D88" s="3" t="s">
@@ -3080,12 +3345,12 @@
       <c r="F88" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G88" s="4">
+      <c r="G88" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="6" t="s">
         <v>233</v>
       </c>
       <c r="D89" s="3" t="s">
@@ -3097,12 +3362,12 @@
       <c r="F89" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G89" s="4">
+      <c r="G89" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="3" t="s">
+      <c r="C90" s="6" t="s">
         <v>227</v>
       </c>
       <c r="D90" s="3" t="s">
@@ -3114,12 +3379,12 @@
       <c r="F90" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G90" s="4">
+      <c r="G90" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="6" t="s">
         <v>231</v>
       </c>
       <c r="D91" s="3" t="s">
@@ -3131,12 +3396,12 @@
       <c r="F91" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G91" s="4" t="s">
+      <c r="G91" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="3" t="s">
+      <c r="C92" s="6" t="s">
         <v>225</v>
       </c>
       <c r="D92" s="3" t="s">
@@ -3148,12 +3413,12 @@
       <c r="F92" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G92" s="4">
+      <c r="G92" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="6" t="s">
         <v>211</v>
       </c>
       <c r="D93" s="3" t="s">
@@ -3165,12 +3430,12 @@
       <c r="F93" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G93" s="4">
+      <c r="G93" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="6" t="s">
         <v>261</v>
       </c>
       <c r="D94" s="3" t="s">
@@ -3182,12 +3447,12 @@
       <c r="F94" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G94" s="4">
+      <c r="G94" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D95" s="3" t="s">
@@ -3199,12 +3464,12 @@
       <c r="F95" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G95" s="4" t="s">
+      <c r="G95" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D96" s="3" t="s">
@@ -3216,12 +3481,12 @@
       <c r="F96" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G96" s="4">
+      <c r="G96" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="6" t="s">
         <v>223</v>
       </c>
       <c r="D97" s="3" t="s">
@@ -3231,12 +3496,12 @@
         <v>263</v>
       </c>
       <c r="F97" s="3"/>
-      <c r="G97" s="4">
+      <c r="G97" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="3" t="s">
+      <c r="C98" s="6" t="s">
         <v>127</v>
       </c>
       <c r="D98" s="3" t="s">
@@ -3246,12 +3511,12 @@
         <v>263</v>
       </c>
       <c r="F98" s="3"/>
-      <c r="G98" s="4">
+      <c r="G98" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C99" s="3" t="s">
+      <c r="C99" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D99" s="3" t="s">
@@ -3263,12 +3528,12 @@
       <c r="F99" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G99" s="4">
+      <c r="G99" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C100" s="3" t="s">
+      <c r="C100" s="6" t="s">
         <v>167</v>
       </c>
       <c r="D100" s="3" t="s">
@@ -3280,12 +3545,12 @@
       <c r="F100" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G100" s="4" t="s">
+      <c r="G100" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C101" s="3" t="s">
+      <c r="C101" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D101" s="3" t="s">
@@ -3297,12 +3562,12 @@
       <c r="F101" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G101" s="4" t="s">
+      <c r="G101" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C102" s="3" t="s">
+      <c r="C102" s="6" t="s">
         <v>71</v>
       </c>
       <c r="D102" s="3" t="s">
@@ -3314,12 +3579,12 @@
       <c r="F102" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G102" s="4">
+      <c r="G102" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C103" s="3" t="s">
+      <c r="C103" s="6" t="s">
         <v>121</v>
       </c>
       <c r="D103" s="3" t="s">
@@ -3331,12 +3596,12 @@
       <c r="F103" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G103" s="4">
+      <c r="G103" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C104" s="3" t="s">
+      <c r="C104" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D104" s="3" t="s">
@@ -3348,12 +3613,12 @@
       <c r="F104" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G104" s="4" t="s">
+      <c r="G104" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C105" s="3" t="s">
+      <c r="C105" s="6" t="s">
         <v>99</v>
       </c>
       <c r="D105" s="3" t="s">
@@ -3365,12 +3630,12 @@
       <c r="F105" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G105" s="4">
+      <c r="G105" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="6" t="s">
         <v>229</v>
       </c>
       <c r="D106" s="3" t="s">
@@ -3382,12 +3647,12 @@
       <c r="F106" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G106" s="4">
+      <c r="G106" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C107" s="3" t="s">
+      <c r="C107" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D107" s="3" t="s">
@@ -3399,12 +3664,12 @@
       <c r="F107" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G107" s="4" t="s">
+      <c r="G107" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C108" s="3" t="s">
+      <c r="C108" s="6" t="s">
         <v>237</v>
       </c>
       <c r="D108" s="3" t="s">
@@ -3416,12 +3681,12 @@
       <c r="F108" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G108" s="4">
+      <c r="G108" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C109" s="3" t="s">
+      <c r="C109" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D109" s="3" t="s">
@@ -3433,12 +3698,12 @@
       <c r="F109" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G109" s="4" t="s">
+      <c r="G109" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="6" t="s">
         <v>115</v>
       </c>
       <c r="D110" s="3" t="s">
@@ -3450,12 +3715,12 @@
       <c r="F110" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G110" s="4" t="s">
+      <c r="G110" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="6" t="s">
         <v>75</v>
       </c>
       <c r="D111" s="3" t="s">
@@ -3467,12 +3732,12 @@
       <c r="F111" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G111" s="4">
+      <c r="G111" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="6" t="s">
         <v>159</v>
       </c>
       <c r="D112" s="3" t="s">
@@ -3484,12 +3749,12 @@
       <c r="F112" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G112" s="4">
+      <c r="G112" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="113" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C113" s="3" t="s">
+      <c r="C113" s="6" t="s">
         <v>197</v>
       </c>
       <c r="D113" s="3" t="s">
@@ -3501,12 +3766,12 @@
       <c r="F113" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G113" s="4">
+      <c r="G113" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="114" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="6" t="s">
         <v>135</v>
       </c>
       <c r="D114" s="3" t="s">
@@ -3518,12 +3783,12 @@
       <c r="F114" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G114" s="4">
+      <c r="G114" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="115" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C115" s="3" t="s">
+      <c r="C115" s="6" t="s">
         <v>247</v>
       </c>
       <c r="D115" s="3" t="s">
@@ -3535,12 +3800,12 @@
       <c r="F115" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G115" s="4">
+      <c r="G115" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="116" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C116" s="3" t="s">
+      <c r="C116" s="6" t="s">
         <v>219</v>
       </c>
       <c r="D116" s="3" t="s">
@@ -3552,12 +3817,12 @@
       <c r="F116" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G116" s="4">
+      <c r="G116" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="117" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C117" s="3" t="s">
+      <c r="C117" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D117" s="3" t="s">
@@ -3569,12 +3834,12 @@
       <c r="F117" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G117" s="4">
+      <c r="G117" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="118" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C118" s="3" t="s">
+      <c r="C118" s="6" t="s">
         <v>85</v>
       </c>
       <c r="D118" s="3" t="s">
@@ -3586,12 +3851,12 @@
       <c r="F118" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G118" s="4" t="s">
+      <c r="G118" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="119" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C119" s="3" t="s">
+      <c r="C119" s="6" t="s">
         <v>243</v>
       </c>
       <c r="D119" s="3" t="s">
@@ -3603,12 +3868,12 @@
       <c r="F119" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G119" s="4">
+      <c r="G119" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C120" s="3" t="s">
+      <c r="C120" s="6" t="s">
         <v>129</v>
       </c>
       <c r="D120" s="3" t="s">
@@ -3620,12 +3885,12 @@
       <c r="F120" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G120" s="4" t="s">
+      <c r="G120" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="121" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C121" s="3" t="s">
+      <c r="C121" s="6" t="s">
         <v>119</v>
       </c>
       <c r="D121" s="3" t="s">
@@ -3635,12 +3900,12 @@
         <v>263</v>
       </c>
       <c r="F121" s="3"/>
-      <c r="G121" s="4">
+      <c r="G121" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="122" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C122" s="3" t="s">
+      <c r="C122" s="6" t="s">
         <v>191</v>
       </c>
       <c r="D122" s="3" t="s">
@@ -3652,12 +3917,12 @@
       <c r="F122" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G122" s="4">
+      <c r="G122" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="123" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C123" s="3" t="s">
+      <c r="C123" s="6" t="s">
         <v>221</v>
       </c>
       <c r="D123" s="3" t="s">
@@ -3669,12 +3934,12 @@
       <c r="F123" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G123" s="4">
+      <c r="G123" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="124" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C124" s="3" t="s">
+      <c r="C124" s="6" t="s">
         <v>264</v>
       </c>
       <c r="D124" s="3" t="s">
@@ -3686,12 +3951,12 @@
       <c r="F124" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G124" s="4">
+      <c r="G124" s="7">
         <v>500</v>
       </c>
     </row>
     <row r="125" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C125" s="3" t="s">
+      <c r="C125" s="6" t="s">
         <v>265</v>
       </c>
       <c r="D125" s="3" t="s">
@@ -3703,12 +3968,12 @@
       <c r="F125" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G125" s="4">
+      <c r="G125" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="126" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C126" s="3" t="s">
+      <c r="C126" s="6" t="s">
         <v>266</v>
       </c>
       <c r="D126" s="3" t="s">
@@ -3720,12 +3985,12 @@
       <c r="F126" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G126" s="4">
+      <c r="G126" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="6" t="s">
         <v>267</v>
       </c>
       <c r="D127" s="3" t="s">
@@ -3737,12 +4002,12 @@
       <c r="F127" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G127" s="4">
+      <c r="G127" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="128" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C128" s="3" t="s">
+      <c r="C128" s="6" t="s">
         <v>268</v>
       </c>
       <c r="D128" s="3" t="s">
@@ -3752,12 +4017,12 @@
         <v>263</v>
       </c>
       <c r="F128" s="3"/>
-      <c r="G128" s="4">
+      <c r="G128" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="129" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C129" s="3" t="s">
+      <c r="C129" s="6" t="s">
         <v>269</v>
       </c>
       <c r="D129" s="3" t="s">
@@ -3769,12 +4034,12 @@
       <c r="F129" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G129" s="4">
+      <c r="G129" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="130" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C130" s="3" t="s">
+      <c r="C130" s="6" t="s">
         <v>139</v>
       </c>
       <c r="D130" s="3" t="s">
@@ -3786,12 +4051,12 @@
       <c r="F130" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G130" s="4" t="s">
+      <c r="G130" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C131" s="3" t="s">
+      <c r="C131" s="6" t="s">
         <v>241</v>
       </c>
       <c r="D131" s="3" t="s">
@@ -3803,12 +4068,12 @@
       <c r="F131" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G131" s="4">
+      <c r="G131" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="132" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C132" s="3" t="s">
+      <c r="C132" s="6" t="s">
         <v>167</v>
       </c>
       <c r="D132" s="3" t="s">
@@ -3820,12 +4085,12 @@
       <c r="F132" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G132" s="4">
+      <c r="G132" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C133" s="3" t="s">
+      <c r="C133" s="6" t="s">
         <v>183</v>
       </c>
       <c r="D133" s="3" t="s">
@@ -3837,25 +4102,39 @@
       <c r="F133" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G133" s="4" t="s">
+      <c r="G133" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="134" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C134" s="3" t="s">
+      <c r="C134" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D134" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="E134" s="3" t="s">
+      <c r="E134" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="F134" s="3" t="s">
+      <c r="F134" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G134" s="4">
+      <c r="G134" s="13">
         <v>500</v>
+      </c>
+    </row>
+    <row r="138" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
+        <v>276</v>
+      </c>
+      <c r="E138">
+        <f>COUNTBLANK(Data[Registration Date])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="139" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -3863,11 +4142,14 @@
     <cfRule type="expression" priority="1" stopIfTrue="1">
       <formula>$S$3=1</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(C5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>